<commit_message>
Ajuste del modelo para su evalucion
</commit_message>
<xml_diff>
--- a/PreparacionDatos/FloraTotal_3mes_3V_mas_4.xlsx
+++ b/PreparacionDatos/FloraTotal_3mes_3V_mas_4.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cristian\Documents\GitHub\LTSM_Cali\PreparacionDatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25055DB6-BECD-48B8-9424-AF98994C2F16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A75689-BC27-4712-B022-FB365889903F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Motos_vehiculos_particulares</t>
   </si>
@@ -39,6 +39,9 @@
   </si>
   <si>
     <t>Poblacion</t>
+  </si>
+  <si>
+    <t>Trimestre</t>
   </si>
 </sst>
 </file>
@@ -97,10 +100,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -440,431 +452,542 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" topLeftCell="B22" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.140625" customWidth="1"/>
-    <col min="2" max="2" width="16.28515625" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" customWidth="1"/>
+    <col min="2" max="2" width="34.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
         <v>348066</v>
       </c>
-      <c r="B2">
+      <c r="C2" s="2">
         <v>0.93961256742477417</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>2244668</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
         <v>348066</v>
       </c>
-      <c r="B3">
+      <c r="C3" s="2">
         <v>0.38281345367431641</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>2244668</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
         <v>348066</v>
       </c>
-      <c r="B4">
+      <c r="C4" s="2">
         <v>0.26317191123962402</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>2244668</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
         <v>348066</v>
       </c>
-      <c r="B5">
+      <c r="C5" s="2">
         <v>0.57283401489257801</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>2244668</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
         <v>391327</v>
       </c>
-      <c r="B6">
+      <c r="C6" s="2">
         <v>0.19038157165050509</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>2269653</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
         <v>391327</v>
       </c>
-      <c r="B7">
+      <c r="C7" s="2">
         <v>0.4135918915271759</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>2269653</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
         <v>391327</v>
       </c>
-      <c r="B8">
+      <c r="C8" s="2">
         <v>0.40893375873565668</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>2269653</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9">
         <v>391327</v>
       </c>
-      <c r="B9">
+      <c r="C9" s="2">
         <v>0.5955079197883606</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>2269653</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
         <v>438769</v>
       </c>
-      <c r="B10">
+      <c r="C10" s="2">
         <v>6.0729164630174637E-2</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>2294653</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11">
         <v>438769</v>
       </c>
-      <c r="B11">
+      <c r="C11" s="2">
         <v>0.42695650458335882</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>2294653</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12">
         <v>438769</v>
       </c>
-      <c r="B12">
+      <c r="C12" s="2">
         <v>0.10770731419324869</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>2294653</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="B13">
         <v>438769</v>
       </c>
-      <c r="B13">
+      <c r="C13" s="2">
         <v>0.41980567574501038</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>2294653</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
         <v>484119</v>
       </c>
-      <c r="B14">
+      <c r="C14" s="2">
         <v>0.18510627746582031</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>2319684</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15">
         <v>484119</v>
       </c>
-      <c r="B15">
+      <c r="C15" s="2">
         <v>0.27611085772514338</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>2319684</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
+        <v>3</v>
+      </c>
+      <c r="B16">
         <v>484119</v>
       </c>
-      <c r="B16">
+      <c r="C16" s="2">
         <v>0.1341729611158371</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>2319684</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
+        <v>4</v>
+      </c>
+      <c r="B17">
         <v>484119</v>
       </c>
-      <c r="B17">
+      <c r="C17" s="2">
         <v>0.47286862134933472</v>
       </c>
-      <c r="C17">
+      <c r="D17">
         <v>2319684</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18">
         <v>526339</v>
       </c>
-      <c r="B18">
+      <c r="C18" s="2">
         <v>0.21564733982086179</v>
       </c>
-      <c r="C18">
+      <c r="D18">
         <v>2344734</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19">
         <v>526339</v>
       </c>
-      <c r="B19">
+      <c r="C19" s="2">
         <v>0.2342570424079895</v>
       </c>
-      <c r="C19">
+      <c r="D19">
         <v>2344734</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="B20">
         <v>526339</v>
       </c>
-      <c r="B20">
+      <c r="C20" s="2">
         <v>0.28155481815338129</v>
       </c>
-      <c r="C20">
+      <c r="D20">
         <v>2344734</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
+        <v>4</v>
+      </c>
+      <c r="B21">
         <v>526339</v>
       </c>
-      <c r="B21">
+      <c r="C21" s="2">
         <v>0.37249055504798889</v>
       </c>
-      <c r="C21">
+      <c r="D21">
         <v>2344734</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22">
         <v>567353</v>
       </c>
-      <c r="B22">
+      <c r="C22" s="2">
         <v>0.20854589343070981</v>
       </c>
-      <c r="C22">
+      <c r="D22">
         <v>2369821</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23">
         <v>567353</v>
       </c>
-      <c r="B23">
+      <c r="C23" s="2">
         <v>0.19350214302539831</v>
       </c>
-      <c r="C23">
+      <c r="D23">
         <v>2369821</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24">
+        <v>3</v>
+      </c>
+      <c r="B24">
         <v>567353</v>
       </c>
-      <c r="B24">
+      <c r="C24" s="2">
         <v>0.1100472584366798</v>
       </c>
-      <c r="C24">
+      <c r="D24">
         <v>2369821</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
+        <v>4</v>
+      </c>
+      <c r="B25">
         <v>567353</v>
       </c>
-      <c r="B25">
+      <c r="C25" s="2">
         <v>0.1241918727755547</v>
       </c>
-      <c r="C25">
+      <c r="D25">
         <v>2369821</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26">
         <v>601794</v>
       </c>
-      <c r="B26">
+      <c r="C26" s="2">
         <v>0.26536071300506592</v>
       </c>
-      <c r="C26">
+      <c r="D26">
         <v>2394925</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
+        <v>2</v>
+      </c>
+      <c r="B27">
         <v>601794</v>
       </c>
-      <c r="B27">
+      <c r="C27" s="2">
         <v>0.25380316376686102</v>
       </c>
-      <c r="C27">
+      <c r="D27">
         <v>2394925</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
+        <v>3</v>
+      </c>
+      <c r="B28">
         <v>601794</v>
       </c>
-      <c r="B28">
+      <c r="C28" s="2">
         <v>8.8913045823574066E-2</v>
       </c>
-      <c r="C28">
+      <c r="D28">
         <v>2394925</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
+        <v>4</v>
+      </c>
+      <c r="B29">
         <v>601794</v>
       </c>
-      <c r="B29">
+      <c r="C29" s="2">
         <v>0.28081285953521729</v>
       </c>
-      <c r="C29">
+      <c r="D29">
         <v>2394925</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="B30">
         <v>630478</v>
       </c>
-      <c r="B30">
+      <c r="C30" s="2">
         <v>1.5700483694672581E-2</v>
       </c>
-      <c r="C30">
+      <c r="D30">
         <v>2420114</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31">
+        <v>2</v>
+      </c>
+      <c r="B31">
         <v>630478</v>
       </c>
-      <c r="B31">
+      <c r="C31" s="2">
         <v>0.181820347905159</v>
       </c>
-      <c r="C31">
+      <c r="D31">
         <v>2420114</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32">
+        <v>3</v>
+      </c>
+      <c r="B32">
         <v>630478</v>
       </c>
-      <c r="B32">
+      <c r="C32" s="2">
         <v>0.1486389487981796</v>
       </c>
-      <c r="C32">
+      <c r="D32">
         <v>2420114</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33">
+        <v>4</v>
+      </c>
+      <c r="B33">
         <v>630478</v>
       </c>
-      <c r="B33">
+      <c r="C33" s="2">
         <v>0.2202126681804657</v>
       </c>
-      <c r="C33">
+      <c r="D33">
         <v>2420114</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
-        <f>A33*9.5</f>
+        <v>1</v>
+      </c>
+      <c r="B34">
+        <f>B33*9.5</f>
         <v>5989541</v>
       </c>
-      <c r="B34">
-        <v>1.5700483694672581E-2</v>
-      </c>
-      <c r="C34">
-        <f>C33*1.07</f>
+      <c r="C34" s="2">
+        <v>0.23297599999999999</v>
+      </c>
+      <c r="D34">
+        <f>D33*1.07</f>
         <v>2589521.98</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
-        <f>A34*0.9</f>
+        <v>2</v>
+      </c>
+      <c r="B35">
+        <f>B34*0.9</f>
         <v>5390586.9000000004</v>
       </c>
-      <c r="B35">
-        <v>0.181820347905159</v>
-      </c>
-      <c r="C35">
-        <f>C33*1.07</f>
+      <c r="C35" s="3">
+        <v>0.28274199999999999</v>
+      </c>
+      <c r="D35">
+        <f>D33*1.07</f>
         <v>2589521.98</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
-        <f>A35*0.85</f>
+        <v>3</v>
+      </c>
+      <c r="B36">
+        <f>B35*0.85</f>
         <v>4581998.8650000002</v>
       </c>
-      <c r="B36">
-        <v>0.1486389487981796</v>
-      </c>
-      <c r="C36">
-        <f>C33*1.07</f>
+      <c r="C36" s="2">
+        <v>0.187975</v>
+      </c>
+      <c r="D36">
+        <f>D33*1.07</f>
         <v>2589521.98</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
-        <f>A36*0.8</f>
+        <v>4</v>
+      </c>
+      <c r="B37">
+        <f>B36*0.8</f>
         <v>3665599.0920000002</v>
       </c>
-      <c r="B37">
-        <v>0.2202126681804657</v>
-      </c>
-      <c r="C37">
-        <f>C33*1.07</f>
+      <c r="C37" s="2">
+        <v>0.36432599999999998</v>
+      </c>
+      <c r="D37">
+        <f>D33*1.07</f>
         <v>2589521.98</v>
       </c>
     </row>

</xml_diff>